<commit_message>
Add roster for ento forms
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/ento_household/forms/ento_household_followup/ento_household_followup.xlsx
+++ b/odkx/app/config/tables/ento_household/forms/ento_household_followup/ento_household_followup.xlsx
@@ -5,14 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="survey" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="choices" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="model" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="settings" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="queries" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="choices" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="model" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="settings" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="prompt_types" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="188">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -53,6 +55,9 @@
     <t xml:space="preserve">display.prompt</t>
   </si>
   <si>
+    <t xml:space="preserve">display.prompt.text</t>
+  </si>
+  <si>
     <t xml:space="preserve">display.hint</t>
   </si>
   <si>
@@ -77,6 +82,27 @@
     <t xml:space="preserve">display.class</t>
   </si>
   <si>
+    <t xml:space="preserve">display.hide_delete_button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.hide_add_instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.hide_edit_button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model.isSessionVariable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter HHID</t>
+  </si>
+  <si>
     <t xml:space="preserve">begin screen</t>
   </si>
   <si>
@@ -113,9 +139,6 @@
     <t xml:space="preserve">selected(data('rand_selected'), 'no')</t>
   </si>
   <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
     <t xml:space="preserve">orig_hh_id</t>
   </si>
   <si>
@@ -158,7 +181,13 @@
     <t xml:space="preserve">qb1.hint</t>
   </si>
   <si>
-    <t xml:space="preserve">// TODO: add roster here</t>
+    <t xml:space="preserve">linked_table_counting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_members_roster_current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roster</t>
   </si>
   <si>
     <t xml:space="preserve">selected(data('qb1'), 'no')</t>
@@ -194,7 +223,10 @@
     <t xml:space="preserve">qb3</t>
   </si>
   <si>
-    <t xml:space="preserve">// TODO: linked mosquito table</t>
+    <t xml:space="preserve">mosquito_net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qb3_count</t>
   </si>
   <si>
     <t xml:space="preserve">qb4</t>
@@ -272,6 +304,72 @@
     <t xml:space="preserve">qc6_length</t>
   </si>
   <si>
+    <t xml:space="preserve">query_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">query_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">callback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_form_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_table_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selectionArgs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_id = ? AND form_status_hh_member_exit IS NOT ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ data('hh_id'), 1 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ento_mosquito_net_followup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ento_mosquito_net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ento_row_id = ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ opendatakit.getCurrentInstanceId() ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ ento_row_id: opendatakit.getCurrentInstanceId(), _locale: getCurrentLocale() }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ _locale: getCurrentLocale() }</t>
+  </si>
+  <si>
     <t xml:space="preserve">choice_list_name</t>
   </si>
   <si>
@@ -416,15 +514,9 @@
     <t xml:space="preserve">absent</t>
   </si>
   <si>
-    <t xml:space="preserve">comment</t>
-  </si>
-  <si>
     <t xml:space="preserve">valuesList</t>
   </si>
   <si>
-    <t xml:space="preserve">hh_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">string</t>
   </si>
   <si>
@@ -495,6 +587,9 @@
   </si>
   <si>
     <t xml:space="preserve">showFooter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prompt_type_name</t>
   </si>
 </sst>
 </file>
@@ -663,12 +758,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:S72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="F71" activeCellId="0" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -678,10 +773,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="13.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="18.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="13.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="18.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="22.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,10 +803,10 @@
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="0" t="s">
         <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -721,575 +818,623 @@
       <c r="L1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N1" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="O1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>17</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>20</v>
+      <c r="A3" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="E10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N14" s="0" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="C16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>40</v>
+      <c r="F20" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>17</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="M24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N24" s="0" t="s">
-        <v>22</v>
+      <c r="A24" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="O25" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>44</v>
+      <c r="C26" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M27" s="0" t="n">
+      <c r="C27" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S27" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="M31" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="M32" s="0" t="s">
-        <v>48</v>
+        <v>58</v>
+      </c>
+      <c r="N32" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="M33" s="0" t="s">
-        <v>48</v>
+        <v>59</v>
+      </c>
+      <c r="N33" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="M39" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
+      </c>
+      <c r="N39" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>56</v>
+      <c r="C44" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="M51" s="0" t="s">
-        <v>62</v>
+        <v>71</v>
+      </c>
+      <c r="N51" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="M53" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="N53" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="G59" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="M59" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N59" s="0" t="s">
-        <v>22</v>
+        <v>76</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="O59" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K70" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="L70" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="L70" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="M70" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="M70" s="0" t="n">
+      <c r="N70" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K71" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="L71" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="L71" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="M71" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="M71" s="0" t="n">
+      <c r="N71" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1304,6 +1449,130 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="45.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.07"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1322,129 +1591,129 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -1455,13 +1724,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
@@ -1469,13 +1738,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1</v>
@@ -1483,13 +1752,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
@@ -1497,13 +1766,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
@@ -1511,13 +1780,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
@@ -1525,13 +1794,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
@@ -1539,13 +1808,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
@@ -1553,13 +1822,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1</v>
@@ -1567,13 +1836,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
@@ -1581,13 +1850,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
@@ -1595,13 +1864,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1</v>
@@ -1609,13 +1878,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>1</v>
@@ -1623,13 +1892,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>1</v>
@@ -1637,13 +1906,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>1</v>
@@ -1651,13 +1920,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>1</v>
@@ -1665,13 +1934,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>1</v>
@@ -1679,13 +1948,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>1</v>
@@ -1693,13 +1962,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>1</v>
@@ -1707,13 +1976,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>1</v>
@@ -1721,13 +1990,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>1</v>
@@ -1735,13 +2004,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>1</v>
@@ -1752,13 +2021,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>1</v>
@@ -1766,13 +2035,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1</v>
@@ -1780,13 +2049,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
@@ -1794,13 +2063,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>1</v>
@@ -1808,13 +2077,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>1</v>
@@ -1822,13 +2091,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>1</v>
@@ -1836,13 +2105,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>1</v>
@@ -1850,13 +2119,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>1</v>
@@ -1864,13 +2133,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>1</v>
@@ -1878,13 +2147,13 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>1</v>
@@ -1892,68 +2161,68 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1967,7 +2236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1987,7 +2256,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>7</v>
@@ -1996,15 +2265,15 @@
         <v>5</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>132</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2018,15 +2287,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2041,41 +2310,41 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20210328001</v>
@@ -2083,79 +2352,119 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>